<commit_message>
feat: enhance chat and dashboard functionalities with daily summaries and improved prompts
</commit_message>
<xml_diff>
--- a/test_results_rag.xlsx
+++ b/test_results_rag.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateu\Documents\SAGEFY\sagefy-functions\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5CD2162-8E83-4B9D-9274-C754F837D758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="811">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="814">
   <si>
     <t>test_id</t>
   </si>
@@ -2833,12 +2839,24 @@
   <si>
     <t>The response is comprehensive and directly addresses the query about the concept of "Tecnologia Social" in the course, providing detailed information without any critical gaps. Thus, it deserves the highest score for adherence.</t>
   </si>
+  <si>
+    <t>MEDIA</t>
+  </si>
+  <si>
+    <t>DESVIO PADRAO</t>
+  </si>
+  <si>
+    <t>TAXA DE SUCESSO</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2854,8 +2872,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2865,6 +2898,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD7E4BC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2893,27 +2932,41 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2951,7 +3004,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -2985,6 +3038,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -3019,9 +3073,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3194,27 +3249,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K101"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="B104" sqref="B104:D104"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="20.7109375" customWidth="1"/>
     <col min="4" max="4" width="22.7109375" customWidth="1"/>
     <col min="5" max="5" width="143.7109375" customWidth="1"/>
     <col min="6" max="6" width="1825.7109375" customWidth="1"/>
     <col min="7" max="7" width="723.7109375" customWidth="1"/>
-    <col min="8" max="8" width="14834.7109375" customWidth="1"/>
+    <col min="8" max="8" width="5472.42578125" customWidth="1"/>
     <col min="9" max="9" width="548.7109375" customWidth="1"/>
     <col min="10" max="10" width="501.7109375" customWidth="1"/>
     <col min="11" max="11" width="411.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3249,7 +3306,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -3284,7 +3341,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -3319,7 +3376,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -3354,7 +3411,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -3389,7 +3446,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -3424,7 +3481,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -3459,7 +3516,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -3494,7 +3551,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -3529,7 +3586,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -3564,7 +3621,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -3599,7 +3656,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -3634,7 +3691,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -3669,7 +3726,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -3704,7 +3761,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -3739,7 +3796,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -3774,7 +3831,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -3809,7 +3866,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -3844,7 +3901,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -3879,7 +3936,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -3914,7 +3971,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -3949,7 +4006,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -3984,7 +4041,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -4019,7 +4076,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -4054,7 +4111,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -4089,7 +4146,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -4124,7 +4181,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -4159,7 +4216,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -4194,7 +4251,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -4229,7 +4286,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -4264,7 +4321,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>40</v>
       </c>
@@ -4299,7 +4356,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>41</v>
       </c>
@@ -4334,7 +4391,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>42</v>
       </c>
@@ -4369,7 +4426,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>43</v>
       </c>
@@ -4404,7 +4461,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>44</v>
       </c>
@@ -4439,7 +4496,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>45</v>
       </c>
@@ -4474,7 +4531,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>46</v>
       </c>
@@ -4509,7 +4566,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>47</v>
       </c>
@@ -4544,7 +4601,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>48</v>
       </c>
@@ -4579,7 +4636,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>49</v>
       </c>
@@ -4614,7 +4671,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>50</v>
       </c>
@@ -4649,7 +4706,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>51</v>
       </c>
@@ -4684,7 +4741,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>52</v>
       </c>
@@ -4719,7 +4776,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>53</v>
       </c>
@@ -4754,7 +4811,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>54</v>
       </c>
@@ -4789,7 +4846,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>55</v>
       </c>
@@ -4824,7 +4881,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>56</v>
       </c>
@@ -4859,7 +4916,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>57</v>
       </c>
@@ -4894,7 +4951,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="49" spans="1:11">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>58</v>
       </c>
@@ -4929,7 +4986,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="50" spans="1:11">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>59</v>
       </c>
@@ -4964,7 +5021,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>60</v>
       </c>
@@ -4999,7 +5056,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>61</v>
       </c>
@@ -5034,7 +5091,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>62</v>
       </c>
@@ -5069,7 +5126,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="54" spans="1:11">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>63</v>
       </c>
@@ -5104,7 +5161,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="55" spans="1:11">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>64</v>
       </c>
@@ -5139,7 +5196,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="56" spans="1:11">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>65</v>
       </c>
@@ -5174,7 +5231,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="57" spans="1:11">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>66</v>
       </c>
@@ -5209,7 +5266,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="58" spans="1:11">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>67</v>
       </c>
@@ -5244,7 +5301,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="59" spans="1:11">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>68</v>
       </c>
@@ -5279,7 +5336,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="60" spans="1:11">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>69</v>
       </c>
@@ -5314,7 +5371,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="61" spans="1:11">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>70</v>
       </c>
@@ -5349,7 +5406,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="62" spans="1:11">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>71</v>
       </c>
@@ -5384,7 +5441,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="63" spans="1:11">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>72</v>
       </c>
@@ -5419,7 +5476,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="64" spans="1:11">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>73</v>
       </c>
@@ -5454,7 +5511,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="65" spans="1:11">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>74</v>
       </c>
@@ -5489,7 +5546,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="66" spans="1:11">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>75</v>
       </c>
@@ -5524,7 +5581,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="67" spans="1:11">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>76</v>
       </c>
@@ -5559,7 +5616,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="68" spans="1:11">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>77</v>
       </c>
@@ -5594,7 +5651,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="69" spans="1:11">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>78</v>
       </c>
@@ -5629,7 +5686,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="70" spans="1:11">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>79</v>
       </c>
@@ -5664,7 +5721,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="71" spans="1:11">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>80</v>
       </c>
@@ -5699,7 +5756,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="72" spans="1:11">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>81</v>
       </c>
@@ -5734,7 +5791,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="73" spans="1:11">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>82</v>
       </c>
@@ -5769,7 +5826,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="74" spans="1:11">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>83</v>
       </c>
@@ -5804,7 +5861,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="75" spans="1:11">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>84</v>
       </c>
@@ -5839,7 +5896,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="76" spans="1:11">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>85</v>
       </c>
@@ -5874,7 +5931,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="77" spans="1:11">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>86</v>
       </c>
@@ -5909,7 +5966,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="78" spans="1:11">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>87</v>
       </c>
@@ -5944,7 +6001,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="79" spans="1:11">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>88</v>
       </c>
@@ -5979,7 +6036,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="80" spans="1:11">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>89</v>
       </c>
@@ -6014,7 +6071,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="81" spans="1:11">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>90</v>
       </c>
@@ -6049,7 +6106,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="82" spans="1:11">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>91</v>
       </c>
@@ -6084,7 +6141,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="83" spans="1:11">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>92</v>
       </c>
@@ -6119,7 +6176,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="84" spans="1:11">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>93</v>
       </c>
@@ -6154,7 +6211,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="85" spans="1:11">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>94</v>
       </c>
@@ -6189,7 +6246,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="86" spans="1:11">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>95</v>
       </c>
@@ -6224,7 +6281,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="87" spans="1:11">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>96</v>
       </c>
@@ -6259,7 +6316,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="88" spans="1:11">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>97</v>
       </c>
@@ -6294,7 +6351,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="89" spans="1:11">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>98</v>
       </c>
@@ -6329,7 +6386,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="90" spans="1:11">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>99</v>
       </c>
@@ -6364,7 +6421,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="91" spans="1:11">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>100</v>
       </c>
@@ -6399,7 +6456,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="92" spans="1:11">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>101</v>
       </c>
@@ -6434,7 +6491,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="93" spans="1:11">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>102</v>
       </c>
@@ -6469,7 +6526,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="94" spans="1:11">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>103</v>
       </c>
@@ -6504,7 +6561,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="95" spans="1:11">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>104</v>
       </c>
@@ -6539,7 +6596,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="96" spans="1:11">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>105</v>
       </c>
@@ -6574,7 +6631,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="97" spans="1:11">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>106</v>
       </c>
@@ -6609,7 +6666,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="98" spans="1:11">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>107</v>
       </c>
@@ -6644,7 +6701,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="99" spans="1:11">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>108</v>
       </c>
@@ -6679,7 +6736,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="100" spans="1:11">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>109</v>
       </c>
@@ -6714,7 +6771,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="101" spans="1:11">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>110</v>
       </c>
@@ -6747,6 +6804,57 @@
       </c>
       <c r="K101" t="s">
         <v>810</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
+        <v>811</v>
+      </c>
+      <c r="B102" s="3">
+        <f>MEDIAN(B2:B101)</f>
+        <v>5</v>
+      </c>
+      <c r="C102" s="3">
+        <f t="shared" ref="C102:D102" si="0">MEDIAN(C2:C101)</f>
+        <v>4</v>
+      </c>
+      <c r="D102" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
+        <v>812</v>
+      </c>
+      <c r="B103" s="3">
+        <f>_xlfn.STDEV.P(B2:B101)</f>
+        <v>0.62120849961989411</v>
+      </c>
+      <c r="C103" s="3">
+        <f t="shared" ref="C103:D103" si="1">_xlfn.STDEV.P(C2:C101)</f>
+        <v>1.0031948963187562</v>
+      </c>
+      <c r="D103" s="3">
+        <f t="shared" si="1"/>
+        <v>1.0049378090210359</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>813</v>
+      </c>
+      <c r="B104" s="3">
+        <f>COUNTIF(B2:B101,"&gt;=4")</f>
+        <v>95</v>
+      </c>
+      <c r="C104" s="3">
+        <f t="shared" ref="C104:D104" si="2">COUNTIF(C2:C101,"&gt;=4")</f>
+        <v>61</v>
+      </c>
+      <c r="D104" s="3">
+        <f t="shared" si="2"/>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>